<commit_message>
Many more edits for clarity and tone.
</commit_message>
<xml_diff>
--- a/full_results_additive-error.xlsx
+++ b/full_results_additive-error.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="13395" windowHeight="6735" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="13395" windowHeight="6735"/>
   </bookViews>
   <sheets>
-    <sheet name="adjustment" sheetId="2" r:id="rId1"/>
-    <sheet name="Egger test" sheetId="3" r:id="rId2"/>
-    <sheet name="dissertation_freqtable" sheetId="4" r:id="rId3"/>
-    <sheet name="full_results" sheetId="1" r:id="rId4"/>
+    <sheet name="adjustment_jeffstyle" sheetId="5" r:id="rId1"/>
+    <sheet name="adjustment" sheetId="2" r:id="rId2"/>
+    <sheet name="Egger test" sheetId="3" r:id="rId3"/>
+    <sheet name="dissertation_freqtable" sheetId="4" r:id="rId4"/>
+    <sheet name="full_results" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="67">
   <si>
     <t>Outcome</t>
   </si>
@@ -216,6 +217,36 @@
   </si>
   <si>
     <t>Publication format</t>
+  </si>
+  <si>
+    <t>Aggressive Affect</t>
+  </si>
+  <si>
+    <t>Aggressive Behavior</t>
+  </si>
+  <si>
+    <t>Aggressive Cognition</t>
+  </si>
+  <si>
+    <t>Experiment - Best</t>
+  </si>
+  <si>
+    <t>Experiment - Full</t>
+  </si>
+  <si>
+    <t>Cross-Section - Best</t>
+  </si>
+  <si>
+    <t>Cross-Section - Full</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -720,7 +751,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -745,6 +776,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -752,6 +786,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1099,10 +1141,569 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.140625" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1318</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <v>0.155033822575671</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-0.12</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>2879</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.217</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>0.164328546161532</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-0.112</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>9811</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
+        <v>0.163590776695582</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0.106</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>2413</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>7.0651304052515504E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.188</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>39</v>
+      </c>
+      <c r="C10">
+        <v>3328</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>5.2187692355472999E-2</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0.127</v>
+      </c>
+      <c r="J10" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>11615</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>0.26716515432230098</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>28337</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>0.226011005235776</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0.152</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>2887</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.217</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.222</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1">
+        <v>0.185129660882245</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.107</v>
+      </c>
+      <c r="J14" s="3">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>4073.5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.216</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1">
+        <v>0.205134435120404</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0.127</v>
+      </c>
+      <c r="J15" s="5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K15">
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>7221</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.184</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
+        <v>0.17207011445932599</v>
+      </c>
+      <c r="I16" s="16">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>12236</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.191</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1">
+        <v>0.16957434468579899</v>
+      </c>
+      <c r="I17" s="16">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J17" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>833</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1">
+        <v>0.26218602019647602</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>1770</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1">
+        <v>0.26864818159793202</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="K20" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A18:K18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K41" sqref="A22:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,17 +1724,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1675,17 +2276,571 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>18</v>
+      </c>
+      <c r="D25">
+        <v>1318</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <v>0.155033822575671</v>
+      </c>
+      <c r="I25" s="1">
+        <v>-0.12</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>2879</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.217</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <v>0.164328546161532</v>
+      </c>
+      <c r="I26" s="1">
+        <v>-0.112</v>
+      </c>
+      <c r="J26" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K26" s="1">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>14</v>
+      </c>
+      <c r="D28">
+        <v>9811</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1">
+        <v>0.163590776695582</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.106</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>23</v>
+      </c>
+      <c r="D30">
+        <v>2413</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1">
+        <v>7.0651304052515504E-2</v>
+      </c>
+      <c r="I30" s="1">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.188</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>39</v>
+      </c>
+      <c r="D31">
+        <v>3328</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1">
+        <v>5.2187692355472999E-2</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.127</v>
+      </c>
+      <c r="J31" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>21</v>
+      </c>
+      <c r="D32">
+        <v>11615</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1">
+        <v>0.26716515432230098</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>36</v>
+      </c>
+      <c r="D33">
+        <v>28337</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1">
+        <v>0.226011005235776</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.152</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>24</v>
+      </c>
+      <c r="D35">
+        <v>2887</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.217</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.222</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1">
+        <v>0.185129660882245</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.107</v>
+      </c>
+      <c r="J35" s="3">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <v>40</v>
+      </c>
+      <c r="D36">
+        <v>4073.5</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.216</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1">
+        <v>0.205134435120404</v>
+      </c>
+      <c r="I36">
+        <v>0.127</v>
+      </c>
+      <c r="J36" s="5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K36">
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>7221</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.184</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1">
+        <v>0.17207011445932599</v>
+      </c>
+      <c r="I37" s="1">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="J37" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38">
+        <v>21</v>
+      </c>
+      <c r="D38">
+        <v>12236</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.191</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1">
+        <v>0.16957434468579899</v>
+      </c>
+      <c r="I38" s="1">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J38" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>833</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1">
+        <v>0.26218602019647602</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41">
+        <v>24</v>
+      </c>
+      <c r="D41">
+        <v>1770</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1">
+        <v>0.26864818159793202</v>
+      </c>
+      <c r="I41" s="1">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="K41" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:L1"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="H22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -2004,11 +3159,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -2023,18 +3178,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2079,10 +3234,10 @@
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2127,19 +3282,19 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2189,10 +3344,10 @@
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2245,7 +3400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF15"/>
   <sheetViews>

</xml_diff>